<commit_message>
added register use cases
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginData.xlsx
+++ b/src/test/resources/LoginData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maya/eclipse-workspace/OrangeHRMTestNG/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C50EC30-6675-3D46-B91A-EF6FFF3C0F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE39FE9-26D9-4F49-8B0D-621401CEF8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17000" xr2:uid="{191F806D-DE8E-7143-9622-866191320E3D}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16980" activeTab="2" xr2:uid="{191F806D-DE8E-7143-9622-866191320E3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Username</t>
   </si>
@@ -79,13 +80,70 @@
   </si>
   <si>
     <t>inline-both</t>
+  </si>
+  <si>
+    <t>TestType</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t>bmiddle</t>
+  </si>
+  <si>
+    <t>blastname</t>
+  </si>
+  <si>
+    <t>Successfully Saved</t>
+  </si>
+  <si>
+    <t>Success Message</t>
+  </si>
+  <si>
+    <t>EmployeeName</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Current Url</t>
+  </si>
+  <si>
+    <t>maya</t>
+  </si>
+  <si>
+    <t>mayababuji</t>
+  </si>
+  <si>
+    <t>@Maya123</t>
+  </si>
+  <si>
+    <t>viewSystemUsers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,6 +157,19 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -122,9 +193,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1274734-7407-5940-AF2B-93D2B404C92F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -470,7 +543,7 @@
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +556,11 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -494,8 +570,11 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -505,8 +584,11 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -519,8 +601,11 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -530,13 +615,19 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -546,56 +637,105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AD71B8-D374-9741-9696-EAFB79271355}">
-  <dimension ref="A2:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D6"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006C1053-0F77-9740-8EE3-294E47BA6844}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>